<commit_message>
Split QO subset to ML + MB
</commit_message>
<xml_diff>
--- a/cns/(cns.generator)/D01A Load Centers - Digest.xlsx
+++ b/cns/(cns.generator)/D01A Load Centers - Digest.xlsx
@@ -12,14 +12,14 @@
     <sheet name="Help" sheetId="2" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Easy Selector Jump Start'!$A$1:$H$86</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Easy Selector Jump Start'!$A$1:$H$278</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2221" uniqueCount="404">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2221" uniqueCount="407">
   <si>
     <t>Catalog#</t>
   </si>
@@ -1231,6 +1231,15 @@
   </si>
   <si>
     <t>D01A</t>
+  </si>
+  <si>
+    <t>Indoor 1Ph3W Main Breaker</t>
+  </si>
+  <si>
+    <t>n/a</t>
+  </si>
+  <si>
+    <t>Indoor 1Ph3W Main Lugs</t>
   </si>
 </sst>
 </file>
@@ -1976,10 +1985,10 @@
   <dimension ref="A1:I278"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D272" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D279" sqref="D279"/>
+      <selection pane="bottomRight" activeCell="D43" sqref="D43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2029,10 +2038,10 @@
         <v>147</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>318</v>
+        <v>404</v>
       </c>
       <c r="E2" s="15" t="s">
-        <v>145</v>
+        <v>405</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>36</v>
@@ -2055,10 +2064,10 @@
         <v>147</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>318</v>
+        <v>404</v>
       </c>
       <c r="E3" s="15" t="s">
-        <v>145</v>
+        <v>405</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>36</v>
@@ -2081,10 +2090,10 @@
         <v>148</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>318</v>
+        <v>404</v>
       </c>
       <c r="E4" s="15" t="s">
-        <v>145</v>
+        <v>405</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>36</v>
@@ -2107,10 +2116,10 @@
         <v>148</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>318</v>
+        <v>404</v>
       </c>
       <c r="E5" s="15" t="s">
-        <v>145</v>
+        <v>405</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>36</v>
@@ -2133,10 +2142,10 @@
         <v>149</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>318</v>
+        <v>404</v>
       </c>
       <c r="E6" s="15" t="s">
-        <v>145</v>
+        <v>405</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>36</v>
@@ -2159,10 +2168,10 @@
         <v>149</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>318</v>
+        <v>404</v>
       </c>
       <c r="E7" s="15" t="s">
-        <v>145</v>
+        <v>405</v>
       </c>
       <c r="F7" s="2" t="s">
         <v>36</v>
@@ -2185,10 +2194,10 @@
         <v>149</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>318</v>
+        <v>404</v>
       </c>
       <c r="E8" s="15" t="s">
-        <v>145</v>
+        <v>405</v>
       </c>
       <c r="F8" s="2" t="s">
         <v>36</v>
@@ -2211,10 +2220,10 @@
         <v>149</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>318</v>
+        <v>404</v>
       </c>
       <c r="E9" s="15" t="s">
-        <v>145</v>
+        <v>405</v>
       </c>
       <c r="F9" s="2" t="s">
         <v>36</v>
@@ -2237,10 +2246,10 @@
         <v>150</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>318</v>
+        <v>404</v>
       </c>
       <c r="E10" s="15" t="s">
-        <v>145</v>
+        <v>405</v>
       </c>
       <c r="F10" s="2" t="s">
         <v>36</v>
@@ -2263,10 +2272,10 @@
         <v>149</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>318</v>
+        <v>404</v>
       </c>
       <c r="E11" s="15" t="s">
-        <v>145</v>
+        <v>405</v>
       </c>
       <c r="F11" s="2" t="s">
         <v>46</v>
@@ -2289,10 +2298,10 @@
         <v>149</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>318</v>
+        <v>404</v>
       </c>
       <c r="E12" s="15" t="s">
-        <v>145</v>
+        <v>405</v>
       </c>
       <c r="F12" s="2" t="s">
         <v>46</v>
@@ -2315,10 +2324,10 @@
         <v>150</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>318</v>
+        <v>404</v>
       </c>
       <c r="E13" s="15" t="s">
-        <v>145</v>
+        <v>405</v>
       </c>
       <c r="F13" s="2" t="s">
         <v>46</v>
@@ -2341,10 +2350,10 @@
         <v>150</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>318</v>
+        <v>404</v>
       </c>
       <c r="E14" s="15" t="s">
-        <v>145</v>
+        <v>405</v>
       </c>
       <c r="F14" s="2" t="s">
         <v>70</v>
@@ -2367,10 +2376,10 @@
         <v>150</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>318</v>
+        <v>404</v>
       </c>
       <c r="E15" s="15" t="s">
-        <v>145</v>
+        <v>405</v>
       </c>
       <c r="F15" s="2" t="s">
         <v>70</v>
@@ -2393,10 +2402,10 @@
         <v>149</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>318</v>
+        <v>404</v>
       </c>
       <c r="E16" s="15" t="s">
-        <v>145</v>
+        <v>405</v>
       </c>
       <c r="F16" s="2" t="s">
         <v>70</v>
@@ -2419,10 +2428,10 @@
         <v>149</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>318</v>
+        <v>404</v>
       </c>
       <c r="E17" s="15" t="s">
-        <v>145</v>
+        <v>405</v>
       </c>
       <c r="F17" s="2" t="s">
         <v>70</v>
@@ -2445,10 +2454,10 @@
         <v>150</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>318</v>
+        <v>404</v>
       </c>
       <c r="E18" s="15" t="s">
-        <v>145</v>
+        <v>405</v>
       </c>
       <c r="F18" s="2" t="s">
         <v>70</v>
@@ -2471,10 +2480,10 @@
         <v>150</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>318</v>
+        <v>404</v>
       </c>
       <c r="E19" s="15" t="s">
-        <v>145</v>
+        <v>405</v>
       </c>
       <c r="F19" s="2" t="s">
         <v>70</v>
@@ -2497,10 +2506,10 @@
         <v>150</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>318</v>
+        <v>404</v>
       </c>
       <c r="E20" s="15" t="s">
-        <v>145</v>
+        <v>405</v>
       </c>
       <c r="F20" s="2" t="s">
         <v>70</v>
@@ -2523,10 +2532,10 @@
         <v>150</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>318</v>
+        <v>404</v>
       </c>
       <c r="E21" s="15" t="s">
-        <v>145</v>
+        <v>405</v>
       </c>
       <c r="F21" s="2" t="s">
         <v>70</v>
@@ -2549,10 +2558,10 @@
         <v>151</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>318</v>
+        <v>404</v>
       </c>
       <c r="E22" s="15" t="s">
-        <v>145</v>
+        <v>405</v>
       </c>
       <c r="F22" s="2" t="s">
         <v>72</v>
@@ -2575,10 +2584,10 @@
         <v>151</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>318</v>
+        <v>404</v>
       </c>
       <c r="E23" s="15" t="s">
-        <v>145</v>
+        <v>405</v>
       </c>
       <c r="F23" s="2" t="s">
         <v>72</v>
@@ -2601,10 +2610,10 @@
         <v>149</v>
       </c>
       <c r="D24" s="8" t="s">
-        <v>318</v>
+        <v>404</v>
       </c>
       <c r="E24" s="15" t="s">
-        <v>145</v>
+        <v>405</v>
       </c>
       <c r="F24" s="2" t="s">
         <v>72</v>
@@ -2627,10 +2636,10 @@
         <v>149</v>
       </c>
       <c r="D25" s="8" t="s">
-        <v>318</v>
+        <v>404</v>
       </c>
       <c r="E25" s="15" t="s">
-        <v>145</v>
+        <v>405</v>
       </c>
       <c r="F25" s="2" t="s">
         <v>72</v>
@@ -2653,10 +2662,10 @@
         <v>150</v>
       </c>
       <c r="D26" s="8" t="s">
-        <v>318</v>
+        <v>404</v>
       </c>
       <c r="E26" s="15" t="s">
-        <v>145</v>
+        <v>405</v>
       </c>
       <c r="F26" s="2" t="s">
         <v>72</v>
@@ -2679,10 +2688,10 @@
         <v>150</v>
       </c>
       <c r="D27" s="8" t="s">
-        <v>318</v>
+        <v>404</v>
       </c>
       <c r="E27" s="15" t="s">
-        <v>145</v>
+        <v>405</v>
       </c>
       <c r="F27" s="2" t="s">
         <v>72</v>
@@ -2705,10 +2714,10 @@
         <v>151</v>
       </c>
       <c r="D28" s="8" t="s">
-        <v>318</v>
+        <v>404</v>
       </c>
       <c r="E28" s="15" t="s">
-        <v>145</v>
+        <v>405</v>
       </c>
       <c r="F28" s="2" t="s">
         <v>72</v>
@@ -2731,10 +2740,10 @@
         <v>151</v>
       </c>
       <c r="D29" s="8" t="s">
-        <v>318</v>
+        <v>404</v>
       </c>
       <c r="E29" s="15" t="s">
-        <v>145</v>
+        <v>405</v>
       </c>
       <c r="F29" s="2" t="s">
         <v>72</v>
@@ -2757,10 +2766,10 @@
         <v>151</v>
       </c>
       <c r="D30" s="8" t="s">
-        <v>318</v>
+        <v>404</v>
       </c>
       <c r="E30" s="15" t="s">
-        <v>145</v>
+        <v>405</v>
       </c>
       <c r="F30" s="2" t="s">
         <v>72</v>
@@ -2783,10 +2792,10 @@
         <v>151</v>
       </c>
       <c r="D31" s="8" t="s">
-        <v>318</v>
+        <v>404</v>
       </c>
       <c r="E31" s="15" t="s">
-        <v>145</v>
+        <v>405</v>
       </c>
       <c r="F31" s="2" t="s">
         <v>72</v>
@@ -2809,10 +2818,10 @@
         <v>151</v>
       </c>
       <c r="D32" s="8" t="s">
-        <v>318</v>
+        <v>404</v>
       </c>
       <c r="E32" s="15" t="s">
-        <v>145</v>
+        <v>405</v>
       </c>
       <c r="F32" s="2" t="s">
         <v>72</v>
@@ -2835,10 +2844,10 @@
         <v>151</v>
       </c>
       <c r="D33" s="8" t="s">
-        <v>318</v>
+        <v>404</v>
       </c>
       <c r="E33" s="15" t="s">
-        <v>145</v>
+        <v>405</v>
       </c>
       <c r="F33" s="2" t="s">
         <v>72</v>
@@ -2861,10 +2870,10 @@
         <v>151</v>
       </c>
       <c r="D34" s="8" t="s">
-        <v>318</v>
+        <v>404</v>
       </c>
       <c r="E34" s="15" t="s">
-        <v>145</v>
+        <v>405</v>
       </c>
       <c r="F34" s="2" t="s">
         <v>72</v>
@@ -2887,10 +2896,10 @@
         <v>151</v>
       </c>
       <c r="D35" s="8" t="s">
-        <v>318</v>
+        <v>404</v>
       </c>
       <c r="E35" s="15" t="s">
-        <v>145</v>
+        <v>405</v>
       </c>
       <c r="F35" s="2" t="s">
         <v>72</v>
@@ -2913,10 +2922,10 @@
         <v>151</v>
       </c>
       <c r="D36" s="8" t="s">
-        <v>318</v>
+        <v>404</v>
       </c>
       <c r="E36" s="15" t="s">
-        <v>145</v>
+        <v>405</v>
       </c>
       <c r="F36" s="2" t="s">
         <v>72</v>
@@ -2939,10 +2948,10 @@
         <v>151</v>
       </c>
       <c r="D37" s="8" t="s">
-        <v>318</v>
+        <v>404</v>
       </c>
       <c r="E37" s="15" t="s">
-        <v>145</v>
+        <v>405</v>
       </c>
       <c r="F37" s="2" t="s">
         <v>72</v>
@@ -2965,10 +2974,10 @@
         <v>151</v>
       </c>
       <c r="D38" s="8" t="s">
-        <v>318</v>
+        <v>404</v>
       </c>
       <c r="E38" s="15" t="s">
-        <v>145</v>
+        <v>405</v>
       </c>
       <c r="F38" s="2" t="s">
         <v>96</v>
@@ -2991,10 +3000,10 @@
         <v>151</v>
       </c>
       <c r="D39" s="8" t="s">
-        <v>318</v>
+        <v>404</v>
       </c>
       <c r="E39" s="15" t="s">
-        <v>145</v>
+        <v>405</v>
       </c>
       <c r="F39" s="2" t="s">
         <v>96</v>
@@ -3017,10 +3026,10 @@
         <v>151</v>
       </c>
       <c r="D40" s="8" t="s">
-        <v>318</v>
+        <v>404</v>
       </c>
       <c r="E40" s="15" t="s">
-        <v>145</v>
+        <v>405</v>
       </c>
       <c r="F40" s="2" t="s">
         <v>96</v>
@@ -3043,10 +3052,10 @@
         <v>151</v>
       </c>
       <c r="D41" s="8" t="s">
-        <v>318</v>
+        <v>404</v>
       </c>
       <c r="E41" s="15" t="s">
-        <v>145</v>
+        <v>405</v>
       </c>
       <c r="F41" s="2" t="s">
         <v>96</v>
@@ -3069,10 +3078,10 @@
         <v>153</v>
       </c>
       <c r="D42" s="8" t="s">
-        <v>318</v>
+        <v>406</v>
       </c>
       <c r="E42" s="15" t="s">
-        <v>144</v>
+        <v>405</v>
       </c>
       <c r="F42" s="2" t="s">
         <v>36</v>
@@ -3095,10 +3104,10 @@
         <v>153</v>
       </c>
       <c r="D43" s="8" t="s">
-        <v>318</v>
+        <v>406</v>
       </c>
       <c r="E43" s="15" t="s">
-        <v>144</v>
+        <v>405</v>
       </c>
       <c r="F43" s="2" t="s">
         <v>36</v>
@@ -3121,10 +3130,10 @@
         <v>153</v>
       </c>
       <c r="D44" s="8" t="s">
-        <v>318</v>
+        <v>406</v>
       </c>
       <c r="E44" s="15" t="s">
-        <v>144</v>
+        <v>405</v>
       </c>
       <c r="F44" s="2" t="s">
         <v>36</v>
@@ -3147,10 +3156,10 @@
         <v>153</v>
       </c>
       <c r="D45" s="8" t="s">
-        <v>318</v>
+        <v>406</v>
       </c>
       <c r="E45" s="15" t="s">
-        <v>144</v>
+        <v>405</v>
       </c>
       <c r="F45" s="2" t="s">
         <v>36</v>
@@ -3173,10 +3182,10 @@
         <v>153</v>
       </c>
       <c r="D46" s="8" t="s">
-        <v>318</v>
+        <v>406</v>
       </c>
       <c r="E46" s="15" t="s">
-        <v>144</v>
+        <v>405</v>
       </c>
       <c r="F46" s="2" t="s">
         <v>36</v>
@@ -3199,10 +3208,10 @@
         <v>153</v>
       </c>
       <c r="D47" s="8" t="s">
-        <v>318</v>
+        <v>406</v>
       </c>
       <c r="E47" s="15" t="s">
-        <v>144</v>
+        <v>405</v>
       </c>
       <c r="F47" s="2" t="s">
         <v>36</v>
@@ -3225,10 +3234,10 @@
         <v>146</v>
       </c>
       <c r="D48" s="8" t="s">
-        <v>318</v>
+        <v>406</v>
       </c>
       <c r="E48" s="15" t="s">
-        <v>144</v>
+        <v>405</v>
       </c>
       <c r="F48" s="2" t="s">
         <v>46</v>
@@ -3251,10 +3260,10 @@
         <v>146</v>
       </c>
       <c r="D49" s="8" t="s">
-        <v>318</v>
+        <v>406</v>
       </c>
       <c r="E49" s="15" t="s">
-        <v>144</v>
+        <v>405</v>
       </c>
       <c r="F49" s="2" t="s">
         <v>46</v>
@@ -3277,10 +3286,10 @@
         <v>146</v>
       </c>
       <c r="D50" s="8" t="s">
-        <v>318</v>
+        <v>406</v>
       </c>
       <c r="E50" s="15" t="s">
-        <v>144</v>
+        <v>405</v>
       </c>
       <c r="F50" s="2" t="s">
         <v>46</v>
@@ -3303,10 +3312,10 @@
         <v>146</v>
       </c>
       <c r="D51" s="8" t="s">
-        <v>318</v>
+        <v>406</v>
       </c>
       <c r="E51" s="15" t="s">
-        <v>144</v>
+        <v>405</v>
       </c>
       <c r="F51" s="2" t="s">
         <v>46</v>
@@ -3329,10 +3338,10 @@
         <v>146</v>
       </c>
       <c r="D52" s="8" t="s">
-        <v>318</v>
+        <v>406</v>
       </c>
       <c r="E52" s="15" t="s">
-        <v>144</v>
+        <v>405</v>
       </c>
       <c r="F52" s="2" t="s">
         <v>46</v>
@@ -3355,10 +3364,10 @@
         <v>146</v>
       </c>
       <c r="D53" s="8" t="s">
-        <v>318</v>
+        <v>406</v>
       </c>
       <c r="E53" s="15" t="s">
-        <v>144</v>
+        <v>405</v>
       </c>
       <c r="F53" s="2" t="s">
         <v>46</v>
@@ -3381,10 +3390,10 @@
         <v>146</v>
       </c>
       <c r="D54" s="8" t="s">
-        <v>318</v>
+        <v>406</v>
       </c>
       <c r="E54" s="15" t="s">
-        <v>144</v>
+        <v>405</v>
       </c>
       <c r="F54" s="2" t="s">
         <v>46</v>
@@ -3407,10 +3416,10 @@
         <v>146</v>
       </c>
       <c r="D55" s="8" t="s">
-        <v>318</v>
+        <v>406</v>
       </c>
       <c r="E55" s="15" t="s">
-        <v>144</v>
+        <v>405</v>
       </c>
       <c r="F55" s="2" t="s">
         <v>46</v>
@@ -3433,10 +3442,10 @@
         <v>146</v>
       </c>
       <c r="D56" s="8" t="s">
-        <v>318</v>
+        <v>406</v>
       </c>
       <c r="E56" s="15" t="s">
-        <v>144</v>
+        <v>405</v>
       </c>
       <c r="F56" s="2" t="s">
         <v>46</v>
@@ -3459,10 +3468,10 @@
         <v>146</v>
       </c>
       <c r="D57" s="8" t="s">
-        <v>318</v>
+        <v>406</v>
       </c>
       <c r="E57" s="15" t="s">
-        <v>144</v>
+        <v>405</v>
       </c>
       <c r="F57" s="2" t="s">
         <v>46</v>
@@ -3485,10 +3494,10 @@
         <v>146</v>
       </c>
       <c r="D58" s="8" t="s">
-        <v>318</v>
+        <v>406</v>
       </c>
       <c r="E58" s="15" t="s">
-        <v>144</v>
+        <v>405</v>
       </c>
       <c r="F58" s="2" t="s">
         <v>46</v>
@@ -3511,10 +3520,10 @@
         <v>146</v>
       </c>
       <c r="D59" s="8" t="s">
-        <v>318</v>
+        <v>406</v>
       </c>
       <c r="E59" s="15" t="s">
-        <v>144</v>
+        <v>405</v>
       </c>
       <c r="F59" s="2" t="s">
         <v>46</v>
@@ -3537,10 +3546,10 @@
         <v>146</v>
       </c>
       <c r="D60" s="8" t="s">
-        <v>318</v>
+        <v>406</v>
       </c>
       <c r="E60" s="15" t="s">
-        <v>144</v>
+        <v>405</v>
       </c>
       <c r="F60" s="2" t="s">
         <v>46</v>
@@ -3563,10 +3572,10 @@
         <v>146</v>
       </c>
       <c r="D61" s="8" t="s">
-        <v>318</v>
+        <v>406</v>
       </c>
       <c r="E61" s="15" t="s">
-        <v>144</v>
+        <v>405</v>
       </c>
       <c r="F61" s="2" t="s">
         <v>46</v>
@@ -3589,10 +3598,10 @@
         <v>146</v>
       </c>
       <c r="D62" s="8" t="s">
-        <v>318</v>
+        <v>406</v>
       </c>
       <c r="E62" s="15" t="s">
-        <v>144</v>
+        <v>405</v>
       </c>
       <c r="F62" s="2" t="s">
         <v>46</v>
@@ -3615,10 +3624,10 @@
         <v>146</v>
       </c>
       <c r="D63" s="8" t="s">
-        <v>318</v>
+        <v>406</v>
       </c>
       <c r="E63" s="15" t="s">
-        <v>144</v>
+        <v>405</v>
       </c>
       <c r="F63" s="2" t="s">
         <v>70</v>
@@ -3641,10 +3650,10 @@
         <v>146</v>
       </c>
       <c r="D64" s="8" t="s">
-        <v>318</v>
+        <v>406</v>
       </c>
       <c r="E64" s="15" t="s">
-        <v>144</v>
+        <v>405</v>
       </c>
       <c r="F64" s="2" t="s">
         <v>70</v>
@@ -3667,10 +3676,10 @@
         <v>146</v>
       </c>
       <c r="D65" s="8" t="s">
-        <v>318</v>
+        <v>406</v>
       </c>
       <c r="E65" s="15" t="s">
-        <v>144</v>
+        <v>405</v>
       </c>
       <c r="F65" s="2" t="s">
         <v>70</v>
@@ -3693,10 +3702,10 @@
         <v>146</v>
       </c>
       <c r="D66" s="8" t="s">
-        <v>318</v>
+        <v>406</v>
       </c>
       <c r="E66" s="15" t="s">
-        <v>144</v>
+        <v>405</v>
       </c>
       <c r="F66" s="2" t="s">
         <v>70</v>
@@ -3719,10 +3728,10 @@
         <v>146</v>
       </c>
       <c r="D67" s="8" t="s">
-        <v>318</v>
+        <v>406</v>
       </c>
       <c r="E67" s="15" t="s">
-        <v>144</v>
+        <v>405</v>
       </c>
       <c r="F67" s="2" t="s">
         <v>70</v>
@@ -3745,10 +3754,10 @@
         <v>146</v>
       </c>
       <c r="D68" s="8" t="s">
-        <v>318</v>
+        <v>406</v>
       </c>
       <c r="E68" s="15" t="s">
-        <v>144</v>
+        <v>405</v>
       </c>
       <c r="F68" s="2" t="s">
         <v>70</v>
@@ -3771,10 +3780,10 @@
         <v>146</v>
       </c>
       <c r="D69" s="8" t="s">
-        <v>318</v>
+        <v>406</v>
       </c>
       <c r="E69" s="15" t="s">
-        <v>144</v>
+        <v>405</v>
       </c>
       <c r="F69" s="2" t="s">
         <v>72</v>
@@ -3797,10 +3806,10 @@
         <v>146</v>
       </c>
       <c r="D70" s="8" t="s">
-        <v>318</v>
+        <v>406</v>
       </c>
       <c r="E70" s="15" t="s">
-        <v>144</v>
+        <v>405</v>
       </c>
       <c r="F70" s="2" t="s">
         <v>72</v>
@@ -3823,10 +3832,10 @@
         <v>146</v>
       </c>
       <c r="D71" s="8" t="s">
-        <v>318</v>
+        <v>406</v>
       </c>
       <c r="E71" s="15" t="s">
-        <v>144</v>
+        <v>405</v>
       </c>
       <c r="F71" s="2" t="s">
         <v>72</v>
@@ -3849,10 +3858,10 @@
         <v>146</v>
       </c>
       <c r="D72" s="8" t="s">
-        <v>318</v>
+        <v>406</v>
       </c>
       <c r="E72" s="15" t="s">
-        <v>144</v>
+        <v>405</v>
       </c>
       <c r="F72" s="2" t="s">
         <v>72</v>
@@ -3875,10 +3884,10 @@
         <v>146</v>
       </c>
       <c r="D73" s="8" t="s">
-        <v>318</v>
+        <v>406</v>
       </c>
       <c r="E73" s="15" t="s">
-        <v>144</v>
+        <v>405</v>
       </c>
       <c r="F73" s="2" t="s">
         <v>72</v>
@@ -3901,10 +3910,10 @@
         <v>146</v>
       </c>
       <c r="D74" s="8" t="s">
-        <v>318</v>
+        <v>406</v>
       </c>
       <c r="E74" s="15" t="s">
-        <v>144</v>
+        <v>405</v>
       </c>
       <c r="F74" s="2" t="s">
         <v>72</v>
@@ -3927,10 +3936,10 @@
         <v>146</v>
       </c>
       <c r="D75" s="8" t="s">
-        <v>318</v>
+        <v>406</v>
       </c>
       <c r="E75" s="15" t="s">
-        <v>144</v>
+        <v>405</v>
       </c>
       <c r="F75" s="2" t="s">
         <v>72</v>
@@ -3953,10 +3962,10 @@
         <v>146</v>
       </c>
       <c r="D76" s="8" t="s">
-        <v>318</v>
+        <v>406</v>
       </c>
       <c r="E76" s="15" t="s">
-        <v>144</v>
+        <v>405</v>
       </c>
       <c r="F76" s="2" t="s">
         <v>72</v>
@@ -3979,10 +3988,10 @@
         <v>146</v>
       </c>
       <c r="D77" s="8" t="s">
-        <v>318</v>
+        <v>406</v>
       </c>
       <c r="E77" s="15" t="s">
-        <v>144</v>
+        <v>405</v>
       </c>
       <c r="F77" s="2" t="s">
         <v>72</v>
@@ -4005,10 +4014,10 @@
         <v>146</v>
       </c>
       <c r="D78" s="8" t="s">
-        <v>318</v>
+        <v>406</v>
       </c>
       <c r="E78" s="15" t="s">
-        <v>144</v>
+        <v>405</v>
       </c>
       <c r="F78" s="2" t="s">
         <v>72</v>
@@ -4031,10 +4040,10 @@
         <v>146</v>
       </c>
       <c r="D79" s="8" t="s">
-        <v>318</v>
+        <v>406</v>
       </c>
       <c r="E79" s="15" t="s">
-        <v>144</v>
+        <v>405</v>
       </c>
       <c r="F79" s="2" t="s">
         <v>72</v>
@@ -4057,10 +4066,10 @@
         <v>146</v>
       </c>
       <c r="D80" s="8" t="s">
-        <v>318</v>
+        <v>406</v>
       </c>
       <c r="E80" s="15" t="s">
-        <v>144</v>
+        <v>405</v>
       </c>
       <c r="F80" s="2" t="s">
         <v>72</v>
@@ -4083,10 +4092,10 @@
         <v>146</v>
       </c>
       <c r="D81" s="8" t="s">
-        <v>318</v>
+        <v>406</v>
       </c>
       <c r="E81" s="15" t="s">
-        <v>144</v>
+        <v>405</v>
       </c>
       <c r="F81" s="2" t="s">
         <v>96</v>
@@ -4109,10 +4118,10 @@
         <v>146</v>
       </c>
       <c r="D82" s="8" t="s">
-        <v>318</v>
+        <v>406</v>
       </c>
       <c r="E82" s="15" t="s">
-        <v>144</v>
+        <v>405</v>
       </c>
       <c r="F82" s="2" t="s">
         <v>96</v>
@@ -4135,10 +4144,10 @@
         <v>152</v>
       </c>
       <c r="D83" s="8" t="s">
-        <v>318</v>
+        <v>406</v>
       </c>
       <c r="E83" s="15" t="s">
-        <v>144</v>
+        <v>405</v>
       </c>
       <c r="F83" s="2" t="s">
         <v>26</v>
@@ -4161,10 +4170,10 @@
         <v>154</v>
       </c>
       <c r="D84" s="8" t="s">
-        <v>318</v>
+        <v>406</v>
       </c>
       <c r="E84" s="15" t="s">
-        <v>144</v>
+        <v>405</v>
       </c>
       <c r="F84" s="2" t="s">
         <v>31</v>
@@ -4187,10 +4196,10 @@
         <v>154</v>
       </c>
       <c r="D85" s="8" t="s">
-        <v>318</v>
+        <v>406</v>
       </c>
       <c r="E85" s="15" t="s">
-        <v>144</v>
+        <v>405</v>
       </c>
       <c r="F85" s="2" t="s">
         <v>31</v>
@@ -4214,10 +4223,10 @@
       </c>
       <c r="C86" s="16"/>
       <c r="D86" s="8" t="s">
-        <v>318</v>
+        <v>406</v>
       </c>
       <c r="E86" s="15" t="s">
-        <v>144</v>
+        <v>405</v>
       </c>
       <c r="F86" s="16" t="s">
         <v>26</v>
@@ -9027,7 +9036,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H86">
+  <autoFilter ref="A1:H278">
     <filterColumn colId="4"/>
   </autoFilter>
   <sortState ref="A2:I91">

</xml_diff>

<commit_message>
unique subset id's to spreadsheets
subset id's must be unique within a spreadsheet
</commit_message>
<xml_diff>
--- a/cns/(cns.generator)/D01A Load Centers - Digest.xlsx
+++ b/cns/(cns.generator)/D01A Load Centers - Digest.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-12" windowWidth="23136" windowHeight="4272" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="-15" windowWidth="23130" windowHeight="4275" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Easy Selector Jump Start" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2441" uniqueCount="440">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2443" uniqueCount="443">
   <si>
     <t>Catalog#</t>
   </si>
@@ -1339,6 +1339,15 @@
   </si>
   <si>
     <t>_17701008</t>
+  </si>
+  <si>
+    <t>_17701008A</t>
+  </si>
+  <si>
+    <t>_17701011A</t>
+  </si>
+  <si>
+    <t>_17701015A</t>
   </si>
 </sst>
 </file>
@@ -2089,14 +2098,14 @@
       <selection pane="bottomRight" activeCell="D293" sqref="D293"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="33" style="2" customWidth="1"/>
-    <col min="2" max="2" width="18.44140625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="18.44140625" style="2" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="49.6640625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="15.109375" style="2" customWidth="1"/>
-    <col min="6" max="8" width="15.6640625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="18.42578125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="18.42578125" style="2" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="49.7109375" style="2" customWidth="1"/>
+    <col min="5" max="5" width="15.140625" style="2" customWidth="1"/>
+    <col min="6" max="8" width="15.7109375" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -9795,16 +9804,16 @@
   <dimension ref="A3:F36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="3" style="11" customWidth="1"/>
     <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="43.88671875" customWidth="1"/>
-    <col min="4" max="4" width="60.6640625" customWidth="1"/>
-    <col min="5" max="6" width="54.6640625" customWidth="1"/>
+    <col min="3" max="3" width="43.85546875" customWidth="1"/>
+    <col min="4" max="4" width="60.7109375" customWidth="1"/>
+    <col min="5" max="6" width="54.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:6">
@@ -9822,7 +9831,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="57.6">
+    <row r="4" spans="1:6" ht="75">
       <c r="A4" s="11" t="s">
         <v>21</v>
       </c>
@@ -9920,7 +9929,7 @@
         <v>22</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="C12" s="8" t="s">
         <v>321</v>
@@ -9976,7 +9985,7 @@
         <v>22</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>434</v>
+        <v>441</v>
       </c>
       <c r="C16" s="8" t="s">
         <v>346</v>
@@ -9986,6 +9995,9 @@
       <c r="F16" s="9"/>
     </row>
     <row r="17" spans="1:6">
+      <c r="A17" s="11" t="s">
+        <v>22</v>
+      </c>
       <c r="B17" s="7" t="s">
         <v>433</v>
       </c>
@@ -9997,8 +10009,11 @@
       <c r="F17" s="9"/>
     </row>
     <row r="18" spans="1:6">
+      <c r="A18" s="11" t="s">
+        <v>22</v>
+      </c>
       <c r="B18" s="7" t="s">
-        <v>433</v>
+        <v>442</v>
       </c>
       <c r="C18" s="17" t="s">
         <v>402</v>
@@ -10210,13 +10225,13 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="12.33203125" customWidth="1"/>
+    <col min="2" max="2" width="12.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:2" ht="15" thickBot="1"/>
-    <row r="2" spans="2:2" ht="15" thickBot="1">
+    <row r="1" spans="2:2" ht="15.75" thickBot="1"/>
+    <row r="2" spans="2:2" ht="15.75" thickBot="1">
       <c r="B2" s="3" t="s">
         <v>2</v>
       </c>

</xml_diff>